<commit_message>
updates of change url button function
</commit_message>
<xml_diff>
--- a/postback_macro.xlsx
+++ b/postback_macro.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gwanggyupark/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gwanggyupark/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64762229-B67B-4540-9BE9-371AB164EBF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDABCC81-CAB8-9248-BD17-37AB2CB8AD73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="500" windowWidth="28300" windowHeight="16100" activeTab="1" xr2:uid="{4173C34D-E5F7-E14F-87C7-069C22F97745}"/>
+    <workbookView xWindow="220" yWindow="500" windowWidth="28300" windowHeight="16100" xr2:uid="{4173C34D-E5F7-E14F-87C7-069C22F97745}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1323,8 +1323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC8A0309-378B-C747-80C1-31F1EC16812B}">
   <dimension ref="A1:H181"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E77" sqref="B1:E77"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="A151" sqref="A78:A151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -2607,7 +2607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4CE521F-33B7-EF4C-BCF5-9E2C7C208F04}">
   <dimension ref="A1:I250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+    <sheetView topLeftCell="A241" workbookViewId="0">
       <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
to show macro list is done
</commit_message>
<xml_diff>
--- a/postback_macro.xlsx
+++ b/postback_macro.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gwanggyupark/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDABCC81-CAB8-9248-BD17-37AB2CB8AD73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187BCBFC-7CEA-2440-B17B-593B6293AE2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="500" windowWidth="28300" windowHeight="16100" xr2:uid="{4173C34D-E5F7-E14F-87C7-069C22F97745}"/>
+    <workbookView xWindow="220" yWindow="500" windowWidth="28300" windowHeight="16100" activeTab="3" xr2:uid="{4173C34D-E5F7-E14F-87C7-069C22F97745}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="437">
   <si>
     <t>{a_key}</t>
   </si>
@@ -919,13 +921,501 @@
   <si>
     <t>{last_deeplink.a_key}</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>애드브릭스가 제공하는 클릭 데이터</t>
+  </si>
+  <si>
+    <t>1530859076437:902a3631-676a-4d57-a428-f7d8962775ad</t>
+  </si>
+  <si>
+    <t>애드브릭스가 제공하는 클릭 쿠키 식별 데이터</t>
+  </si>
+  <si>
+    <t>131bc0bc-ceba-4be9-9aa3-b163d9e5afec</t>
+  </si>
+  <si>
+    <t>애드브릭스가 제공하는 클릭 아이피 데이터</t>
+  </si>
+  <si>
+    <t>14.33.77.170</t>
+  </si>
+  <si>
+    <t>애드브릭스가 제공하는 클릭 핑거프린트 데이터</t>
+  </si>
+  <si>
+    <t>Android 7.0:LG-F800L:14.33.77.170</t>
+  </si>
+  <si>
+    <t>애드브릭스가 제공하는 클릭의 국가 데이터</t>
+  </si>
+  <si>
+    <t>kr</t>
+  </si>
+  <si>
+    <t>애드브릭스가 제공하는 클릭의 도시 데이터</t>
+  </si>
+  <si>
+    <t>suwon-si</t>
+  </si>
+  <si>
+    <t>애드브릭스가 제공하는 클릭의 지역 데이터</t>
+  </si>
+  <si>
+    <t>gyeonggi-do</t>
+  </si>
+  <si>
+    <t>애드브릭스가 제공하는 클릭의 앱키</t>
+  </si>
+  <si>
+    <t>6aE6E7OO5EOsw35P8vCHtQ</t>
+  </si>
+  <si>
+    <t>애드브릭스가 제공하는 클릭의 파트너키</t>
+  </si>
+  <si>
+    <t>WWEzlPofL0CKBJQQLweyHw</t>
+  </si>
+  <si>
+    <t>애드브릭스가 제공하는 클릭의 에이전시 데이터</t>
+  </si>
+  <si>
+    <t>a_agency</t>
+  </si>
+  <si>
+    <t>애드브릭스가 제공하는 클릭의 광고그룹 데이터</t>
+  </si>
+  <si>
+    <t>a_my_adgroup</t>
+  </si>
+  <si>
+    <t>애드브릭스가 제공하는 클릭의 광고</t>
+  </si>
+  <si>
+    <t>a_my_ad</t>
+  </si>
+  <si>
+    <t>애드브릭스가 제공하는 클릭의 캠페인 데이터</t>
+  </si>
+  <si>
+    <t>a_my_campaign</t>
+  </si>
+  <si>
+    <t>애드터치 발생 시각 (애드브릭스 서버 기준)</t>
+  </si>
+  <si>
+    <t>파트너가 전달한 광고물 식별 데이터</t>
+  </si>
+  <si>
+    <t>m_createive_</t>
+  </si>
+  <si>
+    <t>파트너가 전달한 매체 식별 데이터</t>
+  </si>
+  <si>
+    <t>pub_id_120</t>
+  </si>
+  <si>
+    <t>파트너가 전달한 하위 매체 식별 데이터</t>
+  </si>
+  <si>
+    <t>sub_pub_id_980</t>
+  </si>
+  <si>
+    <t>파트너가 전달한 광고 그룹 식별 데이터</t>
+  </si>
+  <si>
+    <t>테스트_한글_광고그룹</t>
+  </si>
+  <si>
+    <t>파트너가 전달한 광고 식별 데이터</t>
+  </si>
+  <si>
+    <t>테스트_한글_광고</t>
+  </si>
+  <si>
+    <t>파트너가 전달한 키워드 식별 데이터</t>
+  </si>
+  <si>
+    <t>테스트_한글_키워드</t>
+  </si>
+  <si>
+    <t>파트너가 전달한 노출 지면 식별 데이터</t>
+  </si>
+  <si>
+    <t>테스트_한글_지역</t>
+  </si>
+  <si>
+    <t>파트너가 전달한 광고 정산 타입</t>
+  </si>
+  <si>
+    <t>파트너가 전달한 광고 예산</t>
+  </si>
+  <si>
+    <t>파트너가 전달한 광고 예산 통화 단위</t>
+  </si>
+  <si>
+    <t>krw</t>
+  </si>
+  <si>
+    <t>파트너가 전달한 광고 재생 퍼센트</t>
+  </si>
+  <si>
+    <t>파트너가 전달한 광고 재생 시간</t>
+  </si>
+  <si>
+    <t>파트너가 전달한 광고 시청 퍼센트</t>
+  </si>
+  <si>
+    <t>파트너가 전달한 광고 시청 시간</t>
+  </si>
+  <si>
+    <t>파트너 클릭 데이터</t>
+  </si>
+  <si>
+    <t>click_data_1</t>
+  </si>
+  <si>
+    <t>click_data_2</t>
+  </si>
+  <si>
+    <t>click_data_3</t>
+  </si>
+  <si>
+    <t>click_data_4</t>
+  </si>
+  <si>
+    <t>click_data_5</t>
+  </si>
+  <si>
+    <t>파트너가 수집하여 전달한 ADID (GAID, IDFA)</t>
+  </si>
+  <si>
+    <t>0fa27c1e-9378-4d1c-8f01-118e094240e5</t>
+  </si>
+  <si>
+    <t>GA 트래킹 데이터</t>
+  </si>
+  <si>
+    <t>utm_source_data</t>
+  </si>
+  <si>
+    <t>utm_medium_data</t>
+  </si>
+  <si>
+    <t>utm_campaign_data</t>
+  </si>
+  <si>
+    <t>utm_data</t>
+  </si>
+  <si>
+    <t>utm_content_data</t>
+  </si>
+  <si>
+    <t>구글광고아이디 or 애플광고식별자</t>
+  </si>
+  <si>
+    <t>애플벤더아이디</t>
+  </si>
+  <si>
+    <t>광고추적제한여부</t>
+  </si>
+  <si>
+    <t>디바이스OS 버전</t>
+  </si>
+  <si>
+    <t>디바이스 모델네임</t>
+  </si>
+  <si>
+    <t>modelmodel</t>
+  </si>
+  <si>
+    <t>디바이스 제조사</t>
+  </si>
+  <si>
+    <t>samsung</t>
+  </si>
+  <si>
+    <t>디바이스 해상도(가로x세로)</t>
+  </si>
+  <si>
+    <t>800x600</t>
+  </si>
+  <si>
+    <t>디바이스 오리엔테이션</t>
+  </si>
+  <si>
+    <t>디바이스 플래폼 / 안드로이드, 아이오에스</t>
+  </si>
+  <si>
+    <t>디바이스 네트워크 타입</t>
+  </si>
+  <si>
+    <t>network</t>
+  </si>
+  <si>
+    <t>디바이스 셀룰러 지원 여부</t>
+  </si>
+  <si>
+    <t>디바이스 통신사</t>
+  </si>
+  <si>
+    <t>skt</t>
+  </si>
+  <si>
+    <t>디바이스 언어</t>
+  </si>
+  <si>
+    <t>디바이스 국가</t>
+  </si>
+  <si>
+    <t>ko</t>
+  </si>
+  <si>
+    <t>디바이스 빌드아이디</t>
+  </si>
+  <si>
+    <t>안드로이드 패키지 네임, 애플 번들 아이디</t>
+  </si>
+  <si>
+    <t>com.adbrix.v2</t>
+  </si>
+  <si>
+    <t>애드브릭스 리마스터 앱키</t>
+  </si>
+  <si>
+    <t>애드브릭스 리마스터 SDK 버전</t>
+  </si>
+  <si>
+    <t>인스톨러 정보</t>
+  </si>
+  <si>
+    <t>google</t>
+  </si>
+  <si>
+    <t>앱 버전</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>어트리뷰션 이벤트 타입</t>
+  </si>
+  <si>
+    <t>하단 어트리뷰션 타입 안내 참고</t>
+  </si>
+  <si>
+    <t>어트리뷰션에 기여한 어트리뷰션 모델 타입</t>
+  </si>
+  <si>
+    <t>하단 어트리뷰션 모델 타입 안내 참고</t>
+  </si>
+  <si>
+    <t>어트리뷰션에 기여한 어트리뷰션 모델명</t>
+  </si>
+  <si>
+    <t>어트리뷰션에 기여한 애드터치 타입</t>
+  </si>
+  <si>
+    <t>하단 애드터치 타입 안내 참고</t>
+  </si>
+  <si>
+    <t>어트리뷰션 이벤트 명</t>
+  </si>
+  <si>
+    <t>abx:firstopen</t>
+  </si>
+  <si>
+    <t>어트리뷰션 유입 여부, 내가 기여한 성과일 때 1을 전달</t>
+  </si>
+  <si>
+    <t>오가닉 유입 여부, 오가닉 유입일 때 1을 전달</t>
+  </si>
+  <si>
+    <t>어트리뷰션 이벤트 발생 시각</t>
+  </si>
+  <si>
+    <t>어트리뷰션 딥링크 정보</t>
+  </si>
+  <si>
+    <t>scheme://host?key=value</t>
+  </si>
+  <si>
+    <t>구글에서 제공하는 설치 버튼 클릭 시각</t>
+  </si>
+  <si>
+    <t>구글에서 제공하는 앱 설치 시작 시각</t>
+  </si>
+  <si>
+    <t>구글에서 제공하는 앱 설치 완료 시각</t>
+  </si>
+  <si>
+    <t>구글에서 제공하는 앱 최초 오픈 시각</t>
+  </si>
+  <si>
+    <t>Click to Install Time</t>
+  </si>
+  <si>
+    <t>이벤트 명</t>
+  </si>
+  <si>
+    <t>이벤트 그룹</t>
+  </si>
+  <si>
+    <t>abx</t>
+  </si>
+  <si>
+    <t>이벤트 발생 시각</t>
+  </si>
+  <si>
+    <t> {req.evt.param_json}</t>
+  </si>
+  <si>
+    <t>커머스이벤트 : 주문번호</t>
+  </si>
+  <si>
+    <t>커머스이벤트 : 주문 총 금액</t>
+  </si>
+  <si>
+    <t>커머스이벤트 : 상품아이디</t>
+  </si>
+  <si>
+    <t>커머스이벤트 : 상품이름</t>
+  </si>
+  <si>
+    <t>여름한정 떨이상품 크록스 20% 할인</t>
+  </si>
+  <si>
+    <t>커머스이벤트 : 상품단가</t>
+  </si>
+  <si>
+    <t>커머스이벤트 : 상품구매수량</t>
+  </si>
+  <si>
+    <t>커머스이벤트 : (단가*수량)-할인</t>
+  </si>
+  <si>
+    <t>커머스이벤트 : 상품할인금액</t>
+  </si>
+  <si>
+    <t>커머스이벤트 : 상품구매통화</t>
+  </si>
+  <si>
+    <t>KRW</t>
+  </si>
+  <si>
+    <t>커머스이벤트 : 상품카테고리정보1</t>
+  </si>
+  <si>
+    <t>기획전</t>
+  </si>
+  <si>
+    <t>a123456789</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>{
+"abx:item.color":"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">메탈블랙",
+"abx:item.abx:product_id":"30290121",
+"abx:item.abx:product_name":"여름한정 떨이상품 크록스 20%할인",
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>"abx:item.abx:price":50000,
+"abx:item.abx:quantity":1,
+"abx:item.abx:discount":10000,
+"abx:item.abx:sales":40000,
+"abx:item.abx:currency":"KRW",
+"abx:item.abx:category1":"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>기획전"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <rFont val="Helvetica"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+}</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이벤트 파라미터(json type)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>a_agency_</t>
+  </si>
+  <si>
+    <t>a_my_adgroup_</t>
+  </si>
+  <si>
+    <t>a_my_ad_</t>
+  </si>
+  <si>
+    <t>a_my_campaign_</t>
+  </si>
+  <si>
+    <t>utm_term_data</t>
+  </si>
+  <si>
+    <t>어트리뷰션이 발생한 adid(GAID, IDFA)</t>
+  </si>
+  <si>
+    <t>45343208-c952-4584-9b60-6f1354a5b9fc</t>
+  </si>
+  <si>
+    <t>어트리뷰션에 기여한 어트리뷰션 모델</t>
+  </si>
+  <si>
+    <t>어트리뷰션이 발생한 시각</t>
+  </si>
+  <si>
+    <t>Click to install time</t>
+  </si>
+  <si>
+    <t>오픈이 발생한 커스텀 딥링크 URL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -951,6 +1441,19 @@
       <sz val="12"/>
       <color rgb="FF333333"/>
       <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Malgun Gothic"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica"/>
       <family val="1"/>
     </font>
   </fonts>
@@ -982,7 +1485,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1005,6 +1508,24 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1323,7 +1844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC8A0309-378B-C747-80C1-31F1EC16812B}">
   <dimension ref="A1:H181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+    <sheetView topLeftCell="A136" workbookViewId="0">
       <selection activeCell="A151" sqref="A78:A151"/>
     </sheetView>
   </sheetViews>
@@ -2607,8 +3128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4CE521F-33B7-EF4C-BCF5-9E2C7C208F04}">
   <dimension ref="A1:I250"/>
   <sheetViews>
-    <sheetView topLeftCell="A241" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -4264,4 +4785,3683 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A994B825-E7E3-3C4C-92E3-F979E61CD077}">
+  <dimension ref="A1:C77"/>
+  <sheetViews>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.5703125" style="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C14" s="9">
+        <v>43641.105358796296</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C15" s="8">
+        <v>1561429903</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C16" s="8">
+        <v>1561429903.6035099</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C24" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C25" s="8">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C27" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C28" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C29" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C30" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C43" s="8"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C44" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C45" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="C49" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C50" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C52" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C56" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C59" s="10">
+        <v>36892</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C67" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C68" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C69" s="9">
+        <v>43641.101354166669</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C70" s="8">
+        <v>1561429557</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C71" s="8">
+        <v>1561429557.747</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C73" s="8">
+        <v>1530859019</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C74" s="8">
+        <v>1530859079</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C75" s="8">
+        <v>1530859079</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="C76" s="8">
+        <v>1530859079</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C77" s="8">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F463018C-7486-374B-8E85-517D780CAFD9}">
+  <dimension ref="A1:G240"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C14" s="9">
+        <v>43641.105358796296</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C15" s="8">
+        <v>1561429903</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C16" s="8">
+        <v>1561429903.6035099</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C24" s="8">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C25" s="8">
+        <v>1000</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" ht="18" customHeight="1">
+      <c r="A26" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C27" s="8">
+        <v>20</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C28" s="8">
+        <v>10</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C29" s="8">
+        <v>10</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C30" s="8">
+        <v>4</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>347</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C43" s="8">
+        <v>1</v>
+      </c>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C47" s="9">
+        <v>43641.105358796296</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C48" s="8">
+        <v>1561429903</v>
+      </c>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C49" s="8">
+        <v>1561429903.6035099</v>
+      </c>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C50" s="8">
+        <v>3</v>
+      </c>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C65" s="9">
+        <v>43641.105358796296</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C66" s="8">
+        <v>1561429903</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C67" s="8">
+        <v>1561429903.6035099</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C75" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C76" s="8">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C78" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C79" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C80" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C81" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C94" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C98" s="9">
+        <v>43641.105358796296</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C99" s="8">
+        <v>1561429903</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C100" s="8">
+        <v>1561429903.6035099</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C101" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C102" s="8" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C104" s="8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C105" s="8" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C106" s="8" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C107" s="8" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C108" s="8" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C109" s="8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C110" s="8" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C111" s="8" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C112" s="8" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C113" s="8" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C114" s="8" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C115" s="8" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C116" s="9">
+        <v>43641.105358796296</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C117" s="8">
+        <v>1561429903</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C118" s="8">
+        <v>1561429903.6035099</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C119" s="8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C120" s="8" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C121" s="8" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C122" s="8" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C123" s="8" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C124" s="8" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C125" s="8" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C126" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C127" s="8">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C128" s="8" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C129" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C130" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C131" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C132" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C133" s="8" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C134" s="8" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C135" s="8" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C136" s="8" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C137" s="8" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C138" s="8" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C139" s="8" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C140" s="8" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C141" s="8" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C142" s="8" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C143" s="8" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C144" s="8" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C145" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C146" s="8" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C147" s="8" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C148" s="8" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C149" s="9">
+        <v>43641.105358796296</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C150" s="8">
+        <v>1561429903</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C151" s="8">
+        <v>1561429903.6035099</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C152" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C153" s="8" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C154" s="8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C155" s="8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C156" s="8" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C157" s="8" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C158" s="8" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C159" s="8" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C160" s="8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C161" s="8" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C162" s="8" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C163" s="8" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C164" s="8" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C165" s="8" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C166" s="8" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="A167" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C167" s="9">
+        <v>43641.105358796296</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C168" s="8">
+        <v>1561429903</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C169" s="8">
+        <v>1561429903.6035099</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C170" s="8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C171" s="8" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C172" s="8" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C173" s="8" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
+      <c r="A174" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C174" s="8" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
+      <c r="A175" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C175" s="8" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="A176" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C176" s="8" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C177" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C178" s="8">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="A179" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C179" s="8" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="A180" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C180" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C181" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C182" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
+      <c r="A183" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C183" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C184" s="8" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="A185" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C185" s="8" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C186" s="8" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C187" s="8" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C188" s="8" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C189" s="8" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C190" s="8" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C191" s="8" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C192" s="8" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C193" s="8" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
+      <c r="A194" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C194" s="8" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
+      <c r="A195" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C195" s="8" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
+      <c r="A196" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C196" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="A197" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C197" s="8" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="A198" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C198" s="8" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C199" s="8" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C200" s="9">
+        <v>43641.105358796296</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C201" s="8">
+        <v>1561429903</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C202" s="8">
+        <v>1561429903.6035099</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C203" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C204" s="8" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="A205" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C205" s="8" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C206" s="8"/>
+    </row>
+    <row r="207" spans="1:3">
+      <c r="A207" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C207" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
+      <c r="A208" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="C208" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
+      <c r="A209" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="C209" s="8" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3">
+      <c r="A210" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C210" s="8" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
+      <c r="A211" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C211" s="8" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3">
+      <c r="A212" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="C212" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3">
+      <c r="A213" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C213" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3">
+      <c r="A214" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C214" s="8" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3">
+      <c r="A215" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C215" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3">
+      <c r="A216" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C216" s="8" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3">
+      <c r="A217" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C217" s="8" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3">
+      <c r="A218" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="C218" s="8" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3">
+      <c r="A219" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C219" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3">
+      <c r="A220" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C220" s="8" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3">
+      <c r="A221" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C221" s="8" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3">
+      <c r="A222" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C222" s="10">
+        <v>36892</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3">
+      <c r="A223" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C223" s="8" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3">
+      <c r="A224" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C224" s="8" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3">
+      <c r="A225" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="C225" s="8" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3">
+      <c r="A226" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="C226" s="8" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3">
+      <c r="A227" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C227" s="9">
+        <v>43641.105358796296</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3">
+      <c r="A228" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C228" s="8">
+        <v>1561429903</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3">
+      <c r="A229" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C229" s="8">
+        <v>1561429903.6035099</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" ht="195">
+      <c r="A230" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B230" s="13" t="s">
+        <v>425</v>
+      </c>
+      <c r="C230" s="12" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3">
+      <c r="A231" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="C231" s="8" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3">
+      <c r="A232" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="C232" s="8">
+        <v>299000</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3">
+      <c r="A233" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="C233" s="8">
+        <v>30290121</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3">
+      <c r="A234" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="C234" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3">
+      <c r="A235" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C235" s="8">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3">
+      <c r="A236" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="C236" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3">
+      <c r="A237" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="C237" s="8">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3">
+      <c r="A238" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="C238" s="8">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3">
+      <c r="A239" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C239" s="8" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3">
+      <c r="A240" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C240" s="8" t="s">
+        <v>422</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
show description of macro
</commit_message>
<xml_diff>
--- a/postback_macro.xlsx
+++ b/postback_macro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gwanggyupark/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187BCBFC-7CEA-2440-B17B-593B6293AE2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0FBDE2-21AC-8949-AC7B-5DE9E2E0F205}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="220" yWindow="500" windowWidth="28300" windowHeight="16100" activeTab="3" xr2:uid="{4173C34D-E5F7-E14F-87C7-069C22F97745}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="488">
   <si>
     <t>{a_key}</t>
   </si>
@@ -1266,9 +1266,6 @@
   </si>
   <si>
     <t>이벤트 발생 시각</t>
-  </si>
-  <si>
-    <t> {req.evt.param_json}</t>
   </si>
   <si>
     <t>커머스이벤트 : 주문번호</t>
@@ -1409,6 +1406,163 @@
   </si>
   <si>
     <t>오픈이 발생한 커스텀 딥링크 URL</t>
+  </si>
+  <si>
+    <t>apple vendor id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{attribution_type.a_key}</t>
+  </si>
+  <si>
+    <t>{attribution_type.a_cookie}</t>
+  </si>
+  <si>
+    <t>{attribution_type.a_ip}</t>
+  </si>
+  <si>
+    <t>{attribution_type.a_fp}</t>
+  </si>
+  <si>
+    <t>{attribution_type.a_country}</t>
+  </si>
+  <si>
+    <t>{attribution_type.a_city}</t>
+  </si>
+  <si>
+    <t>{attribution_type.a_region}</t>
+  </si>
+  <si>
+    <t>{attribution_type.a_appkey}</t>
+  </si>
+  <si>
+    <t>{attribution_type.a_partner}</t>
+  </si>
+  <si>
+    <t>{attribution_type.a_agency}</t>
+  </si>
+  <si>
+    <t>{attribution_type.a_my_adgroup}</t>
+  </si>
+  <si>
+    <t>{attribution_type.a_my_ad}</t>
+  </si>
+  <si>
+    <t>{attribution_type.a_my_campaign}</t>
+  </si>
+  <si>
+    <t>{attribution_type.a_adtouch_datetime}</t>
+  </si>
+  <si>
+    <t>{attribution_type.a_adtouch_timestamp}</t>
+  </si>
+  <si>
+    <t>{attribution_type.a_adtouch_timestamp_d}</t>
+  </si>
+  <si>
+    <t>{attribution_type.m_creative}</t>
+  </si>
+  <si>
+    <t>{attribution_type.m_publisher}</t>
+  </si>
+  <si>
+    <t>{attribution_type.m_sub_publisher}</t>
+  </si>
+  <si>
+    <t>{attribution_type.m_adgroup}</t>
+  </si>
+  <si>
+    <t>{attribution_type.m_ad}</t>
+  </si>
+  <si>
+    <t>{attribution_type.m_keyword}</t>
+  </si>
+  <si>
+    <t>{attribution_type.m_placement}</t>
+  </si>
+  <si>
+    <t>{attribution_type.m_cost_model}</t>
+  </si>
+  <si>
+    <t>{attribution_type.m_cost}</t>
+  </si>
+  <si>
+    <t>{attribution_type.m_cost_currency}</t>
+  </si>
+  <si>
+    <t>{attribution_type.m_play_percent}</t>
+  </si>
+  <si>
+    <t>{attribution_type.m_play_second}</t>
+  </si>
+  <si>
+    <t>{attribution_type.m_view_percent}</t>
+  </si>
+  <si>
+    <t>{attribution_type.m_view_second}</t>
+  </si>
+  <si>
+    <t>{attribution_type.cb_1}</t>
+  </si>
+  <si>
+    <t>{attribution_type.cb_2}</t>
+  </si>
+  <si>
+    <t>{attribution_type.cb_3}</t>
+  </si>
+  <si>
+    <t>{attribution_type.cb_4}</t>
+  </si>
+  <si>
+    <t>{attribution_type.cb_5}</t>
+  </si>
+  <si>
+    <t>{attribution_type.m_adid}</t>
+  </si>
+  <si>
+    <t>{attribution_type.utm_source}</t>
+  </si>
+  <si>
+    <t>{attribution_type.utm_medium}</t>
+  </si>
+  <si>
+    <t>{attribution_type.utm_campaign}</t>
+  </si>
+  <si>
+    <t>{attribution_type.utm_term}</t>
+  </si>
+  <si>
+    <t>{attribution_type.utm_content}</t>
+  </si>
+  <si>
+    <t>{attribution_type.adid}</t>
+  </si>
+  <si>
+    <t>{attribution_type.is_attr_owner}</t>
+  </si>
+  <si>
+    <t>{attribution_type.attr_model_flag}</t>
+  </si>
+  <si>
+    <t>{attribution_type.attr_model_str}</t>
+  </si>
+  <si>
+    <t>{attribution_type.i_request_type}</t>
+  </si>
+  <si>
+    <t>{attribution_type.attribute_datetime}</t>
+  </si>
+  <si>
+    <t>{attribution_type.attribute_timestamp}</t>
+  </si>
+  <si>
+    <t>{attribution_type.attribute_timestamp_d}</t>
+  </si>
+  <si>
+    <t>{attribution_type.seconds_gap}</t>
+  </si>
+  <si>
+    <t>{attribution_type.deeplink_custom_path}</t>
   </si>
 </sst>
 </file>
@@ -1485,7 +1639,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1527,6 +1681,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3128,7 +3291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4CE521F-33B7-EF4C-BCF5-9E2C7C208F04}">
   <dimension ref="A1:I250"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A85" workbookViewId="0">
       <selection sqref="A1:A204"/>
     </sheetView>
   </sheetViews>
@@ -4791,8 +4954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A994B825-E7E3-3C4C-92E3-F979E61CD077}">
   <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -5271,7 +5434,9 @@
       <c r="B43" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="C43" s="8"/>
+      <c r="C43" s="8" t="s">
+        <v>436</v>
+      </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="1" t="s">
@@ -5655,10 +5820,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F463018C-7486-374B-8E85-517D780CAFD9}">
-  <dimension ref="A1:G240"/>
+  <dimension ref="A1:G204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -5671,7 +5836,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="5" t="s">
-        <v>127</v>
+        <v>437</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>294</v>
@@ -5685,7 +5850,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>128</v>
+        <v>438</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>296</v>
@@ -5699,7 +5864,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>129</v>
+        <v>439</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>298</v>
@@ -5713,7 +5878,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>130</v>
+        <v>440</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>300</v>
@@ -5727,7 +5892,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>131</v>
+        <v>441</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>302</v>
@@ -5741,7 +5906,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>84</v>
+        <v>442</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>304</v>
@@ -5755,7 +5920,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>85</v>
+        <v>443</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>306</v>
@@ -5769,7 +5934,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>86</v>
+        <v>444</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>308</v>
@@ -5783,7 +5948,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>87</v>
+        <v>445</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>310</v>
@@ -5797,13 +5962,13 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>88</v>
+        <v>446</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>312</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -5811,13 +5976,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>89</v>
+        <v>447</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>314</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -5825,13 +5990,13 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>90</v>
+        <v>448</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>316</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -5839,13 +6004,13 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>91</v>
+        <v>449</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>318</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -5853,7 +6018,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>92</v>
+        <v>450</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>320</v>
@@ -5867,7 +6032,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
-        <v>93</v>
+        <v>451</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>320</v>
@@ -5881,7 +6046,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>94</v>
+        <v>452</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>320</v>
@@ -5895,7 +6060,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
-        <v>277</v>
+        <v>453</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>321</v>
@@ -5909,7 +6074,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
-        <v>95</v>
+        <v>454</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>323</v>
@@ -5923,7 +6088,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
-        <v>96</v>
+        <v>455</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>325</v>
@@ -5937,7 +6102,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="1" t="s">
-        <v>97</v>
+        <v>456</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>327</v>
@@ -5951,7 +6116,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="1" t="s">
-        <v>98</v>
+        <v>457</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>329</v>
@@ -5965,7 +6130,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="1" t="s">
-        <v>99</v>
+        <v>458</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>331</v>
@@ -5979,7 +6144,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
-        <v>100</v>
+        <v>459</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>333</v>
@@ -5993,7 +6158,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
-        <v>101</v>
+        <v>460</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>335</v>
@@ -6007,7 +6172,7 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="1" t="s">
-        <v>102</v>
+        <v>461</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>336</v>
@@ -6021,7 +6186,7 @@
     </row>
     <row r="26" spans="1:7" ht="18" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>103</v>
+        <v>462</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>337</v>
@@ -6035,7 +6200,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="1" t="s">
-        <v>104</v>
+        <v>463</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>339</v>
@@ -6049,7 +6214,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="1" t="s">
-        <v>105</v>
+        <v>464</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>340</v>
@@ -6063,7 +6228,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="1" t="s">
-        <v>106</v>
+        <v>465</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>341</v>
@@ -6077,7 +6242,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="1" t="s">
-        <v>107</v>
+        <v>466</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>342</v>
@@ -6091,7 +6256,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="1" t="s">
-        <v>108</v>
+        <v>467</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>343</v>
@@ -6105,7 +6270,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="1" t="s">
-        <v>109</v>
+        <v>468</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>343</v>
@@ -6119,7 +6284,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="1" t="s">
-        <v>110</v>
+        <v>469</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>343</v>
@@ -6133,7 +6298,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="1" t="s">
-        <v>111</v>
+        <v>470</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>343</v>
@@ -6147,7 +6312,7 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="1" t="s">
-        <v>112</v>
+        <v>471</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>343</v>
@@ -6161,7 +6326,7 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="1" t="s">
-        <v>113</v>
+        <v>472</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>349</v>
@@ -6175,7 +6340,7 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="1" t="s">
-        <v>278</v>
+        <v>473</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>351</v>
@@ -6189,7 +6354,7 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="1" t="s">
-        <v>114</v>
+        <v>474</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>351</v>
@@ -6203,7 +6368,7 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="1" t="s">
-        <v>115</v>
+        <v>475</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>351</v>
@@ -6217,13 +6382,13 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="1" t="s">
-        <v>116</v>
+        <v>476</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>351</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -6231,7 +6396,7 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="1" t="s">
-        <v>117</v>
+        <v>477</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>351</v>
@@ -6245,13 +6410,13 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="1" t="s">
-        <v>279</v>
+        <v>478</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="C42" s="8" t="s">
         <v>431</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>432</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -6259,7 +6424,7 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="1" t="s">
-        <v>118</v>
+        <v>479</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>395</v>
@@ -6273,10 +6438,10 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="1" t="s">
-        <v>119</v>
+        <v>480</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>389</v>
@@ -6287,7 +6452,7 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="1" t="s">
-        <v>120</v>
+        <v>481</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>390</v>
@@ -6301,7 +6466,7 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="1" t="s">
-        <v>121</v>
+        <v>482</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>391</v>
@@ -6315,10 +6480,10 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="1" t="s">
-        <v>122</v>
+        <v>483</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C47" s="9">
         <v>43641.105358796296</v>
@@ -6329,10 +6494,10 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="1" t="s">
-        <v>123</v>
+        <v>484</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C48" s="8">
         <v>1561429903</v>
@@ -6343,10 +6508,10 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="1" t="s">
-        <v>124</v>
+        <v>485</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C49" s="8">
         <v>1561429903.6035099</v>
@@ -6357,10 +6522,10 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="1" t="s">
-        <v>125</v>
+        <v>486</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C50" s="8">
         <v>3</v>
@@ -6371,10 +6536,10 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="1" t="s">
-        <v>126</v>
+        <v>487</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>399</v>
@@ -6384,2081 +6549,983 @@
       <c r="G51" s="1"/>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="5" t="s">
-        <v>132</v>
+      <c r="A52" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>294</v>
+        <v>357</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>295</v>
+        <v>350</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="1" t="s">
-        <v>133</v>
+        <v>39</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>297</v>
-      </c>
+        <v>358</v>
+      </c>
+      <c r="C53" s="8"/>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="1" t="s">
-        <v>134</v>
+        <v>40</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>299</v>
+        <v>359</v>
+      </c>
+      <c r="C54" s="8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="1" t="s">
-        <v>135</v>
+        <v>41</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>301</v>
+        <v>360</v>
+      </c>
+      <c r="C55" s="8">
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="1" t="s">
-        <v>136</v>
+        <v>42</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>302</v>
+        <v>361</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>303</v>
+        <v>362</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="1" t="s">
-        <v>137</v>
+        <v>43</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>304</v>
+        <v>363</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>305</v>
+        <v>364</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="1" t="s">
-        <v>138</v>
+        <v>44</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>306</v>
+        <v>365</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>307</v>
+        <v>366</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="1" t="s">
-        <v>139</v>
+        <v>45</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>309</v>
+        <v>367</v>
+      </c>
+      <c r="C59" s="8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="1" t="s">
-        <v>140</v>
+        <v>46</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>311</v>
+        <v>368</v>
+      </c>
+      <c r="C60" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="1" t="s">
-        <v>141</v>
+        <v>47</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>312</v>
+        <v>369</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>426</v>
+        <v>370</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="1" t="s">
-        <v>142</v>
+        <v>48</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>427</v>
+        <v>371</v>
+      </c>
+      <c r="C62" s="8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="1" t="s">
-        <v>143</v>
+        <v>49</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>316</v>
+        <v>372</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>428</v>
+        <v>373</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="1" t="s">
-        <v>144</v>
+        <v>50</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>318</v>
+        <v>374</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>429</v>
+        <v>303</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="1" t="s">
-        <v>145</v>
+        <v>51</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="C65" s="9">
-        <v>43641.105358796296</v>
+        <v>375</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="1" t="s">
-        <v>146</v>
+        <v>52</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>320</v>
+        <v>377</v>
       </c>
       <c r="C66" s="8">
-        <v>1561429903</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="1" t="s">
-        <v>147</v>
+        <v>275</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="C67" s="8">
-        <v>1561429903.6035099</v>
+        <v>378</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="1" t="s">
-        <v>280</v>
+        <v>53</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>321</v>
+        <v>380</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="1" t="s">
-        <v>148</v>
+        <v>54</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C69" s="8" t="s">
-        <v>324</v>
+        <v>381</v>
+      </c>
+      <c r="C69" s="10">
+        <v>36892</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="1" t="s">
-        <v>149</v>
+        <v>55</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>325</v>
+        <v>382</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>326</v>
+        <v>383</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="1" t="s">
-        <v>150</v>
+        <v>56</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>327</v>
+        <v>384</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>328</v>
+        <v>385</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="1" t="s">
-        <v>151</v>
+        <v>276</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>329</v>
+        <v>405</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>330</v>
+        <v>394</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="1" t="s">
-        <v>152</v>
+        <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>331</v>
+        <v>406</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>332</v>
+        <v>407</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="1" t="s">
-        <v>153</v>
+        <v>63</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C74" s="8" t="s">
-        <v>334</v>
+        <v>408</v>
+      </c>
+      <c r="C74" s="9">
+        <v>43641.105358796296</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="1" t="s">
-        <v>154</v>
+        <v>64</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>335</v>
+        <v>408</v>
       </c>
       <c r="C75" s="8">
-        <v>0</v>
+        <v>1561429903</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="1" t="s">
-        <v>155</v>
+        <v>65</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>336</v>
+        <v>408</v>
       </c>
       <c r="C76" s="8">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>338</v>
+        <v>1561429903.6035099</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="195">
+      <c r="A77" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B77" s="13" t="s">
+        <v>424</v>
+      </c>
+      <c r="C77" s="12" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="1" t="s">
-        <v>157</v>
+        <v>73</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="C78" s="8">
-        <v>20</v>
+        <v>409</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="1" t="s">
-        <v>158</v>
+        <v>74</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>340</v>
+        <v>410</v>
       </c>
       <c r="C79" s="8">
-        <v>10</v>
+        <v>299000</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="1" t="s">
-        <v>159</v>
+        <v>75</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>341</v>
+        <v>411</v>
       </c>
       <c r="C80" s="8">
-        <v>10</v>
+        <v>30290121</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="1" t="s">
-        <v>160</v>
+        <v>76</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="C81" s="8">
-        <v>4</v>
+        <v>412</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="1" t="s">
-        <v>161</v>
+        <v>77</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>344</v>
+        <v>414</v>
+      </c>
+      <c r="C82" s="8">
+        <v>50000</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="1" t="s">
-        <v>162</v>
+        <v>78</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>345</v>
+        <v>415</v>
+      </c>
+      <c r="C83" s="8">
+        <v>10</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="1" t="s">
-        <v>163</v>
+        <v>79</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>346</v>
+        <v>416</v>
+      </c>
+      <c r="C84" s="8">
+        <v>40000</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="1" t="s">
-        <v>164</v>
+        <v>80</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="C85" s="8" t="s">
-        <v>347</v>
+        <v>417</v>
+      </c>
+      <c r="C85" s="8">
+        <v>10000</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="1" t="s">
-        <v>165</v>
+        <v>81</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>343</v>
+        <v>418</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>348</v>
+        <v>419</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="1" t="s">
-        <v>166</v>
+        <v>82</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>349</v>
+        <v>420</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>350</v>
+        <v>421</v>
       </c>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C88" s="8" t="s">
-        <v>352</v>
-      </c>
+      <c r="A88" s="14"/>
+      <c r="B88" s="14"/>
+      <c r="C88" s="15"/>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>353</v>
-      </c>
+      <c r="A89" s="14"/>
+      <c r="B89" s="14"/>
+      <c r="C89" s="15"/>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C90" s="8" t="s">
-        <v>354</v>
-      </c>
+      <c r="A90" s="14"/>
+      <c r="B90" s="14"/>
+      <c r="C90" s="15"/>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C91" s="8" t="s">
-        <v>430</v>
-      </c>
+      <c r="A91" s="14"/>
+      <c r="B91" s="14"/>
+      <c r="C91" s="15"/>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C92" s="8" t="s">
-        <v>356</v>
-      </c>
+      <c r="A92" s="14"/>
+      <c r="B92" s="14"/>
+      <c r="C92" s="15"/>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="C93" s="8" t="s">
-        <v>432</v>
-      </c>
+      <c r="A93" s="14"/>
+      <c r="B93" s="14"/>
+      <c r="C93" s="15"/>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="C94" s="8">
-        <v>1</v>
-      </c>
+      <c r="A94" s="14"/>
+      <c r="B94" s="14"/>
+      <c r="C94" s="15"/>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="C95" s="8" t="s">
-        <v>389</v>
-      </c>
+      <c r="A95" s="14"/>
+      <c r="B95" s="14"/>
+      <c r="C95" s="15"/>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="C96" s="8" t="s">
-        <v>389</v>
-      </c>
+      <c r="A96" s="14"/>
+      <c r="B96" s="14"/>
+      <c r="C96" s="15"/>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="C97" s="8" t="s">
-        <v>392</v>
-      </c>
+      <c r="A97" s="14"/>
+      <c r="B97" s="14"/>
+      <c r="C97" s="15"/>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="C98" s="9">
-        <v>43641.105358796296</v>
-      </c>
+      <c r="A98" s="14"/>
+      <c r="B98" s="14"/>
+      <c r="C98" s="16"/>
     </row>
     <row r="99" spans="1:3">
-      <c r="A99" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="C99" s="8">
-        <v>1561429903</v>
-      </c>
+      <c r="A99" s="14"/>
+      <c r="B99" s="14"/>
+      <c r="C99" s="15"/>
     </row>
     <row r="100" spans="1:3">
-      <c r="A100" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="C100" s="8">
-        <v>1561429903.6035099</v>
-      </c>
+      <c r="A100" s="14"/>
+      <c r="B100" s="14"/>
+      <c r="C100" s="15"/>
     </row>
     <row r="101" spans="1:3">
-      <c r="A101" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="C101" s="8">
-        <v>3</v>
-      </c>
+      <c r="A101" s="14"/>
+      <c r="B101" s="14"/>
+      <c r="C101" s="15"/>
     </row>
     <row r="102" spans="1:3">
-      <c r="A102" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="C102" s="8" t="s">
-        <v>399</v>
-      </c>
+      <c r="A102" s="14"/>
+      <c r="B102" s="14"/>
+      <c r="C102" s="15"/>
     </row>
     <row r="103" spans="1:3">
-      <c r="A103" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="C103" s="8" t="s">
-        <v>295</v>
-      </c>
+      <c r="A103" s="14"/>
+      <c r="B103" s="14"/>
+      <c r="C103" s="15"/>
     </row>
     <row r="104" spans="1:3">
-      <c r="A104" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="C104" s="8" t="s">
-        <v>297</v>
-      </c>
+      <c r="A104" s="14"/>
+      <c r="B104" s="14"/>
+      <c r="C104" s="15"/>
     </row>
     <row r="105" spans="1:3">
-      <c r="A105" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="C105" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="A105" s="14"/>
+      <c r="B105" s="14"/>
+      <c r="C105" s="15"/>
     </row>
     <row r="106" spans="1:3">
-      <c r="A106" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="C106" s="8" t="s">
-        <v>301</v>
-      </c>
+      <c r="A106" s="14"/>
+      <c r="B106" s="14"/>
+      <c r="C106" s="15"/>
     </row>
     <row r="107" spans="1:3">
-      <c r="A107" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="C107" s="8" t="s">
-        <v>303</v>
-      </c>
+      <c r="A107" s="14"/>
+      <c r="B107" s="14"/>
+      <c r="C107" s="15"/>
     </row>
     <row r="108" spans="1:3">
-      <c r="A108" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="C108" s="8" t="s">
-        <v>305</v>
-      </c>
+      <c r="A108" s="14"/>
+      <c r="B108" s="14"/>
+      <c r="C108" s="15"/>
     </row>
     <row r="109" spans="1:3">
-      <c r="A109" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="C109" s="8" t="s">
-        <v>307</v>
-      </c>
+      <c r="A109" s="14"/>
+      <c r="B109" s="14"/>
+      <c r="C109" s="15"/>
     </row>
     <row r="110" spans="1:3">
-      <c r="A110" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="C110" s="8" t="s">
-        <v>309</v>
-      </c>
+      <c r="A110" s="14"/>
+      <c r="B110" s="14"/>
+      <c r="C110" s="15"/>
     </row>
     <row r="111" spans="1:3">
-      <c r="A111" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="C111" s="8" t="s">
-        <v>311</v>
-      </c>
+      <c r="A111" s="14"/>
+      <c r="B111" s="14"/>
+      <c r="C111" s="15"/>
     </row>
     <row r="112" spans="1:3">
-      <c r="A112" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C112" s="8" t="s">
-        <v>426</v>
-      </c>
+      <c r="A112" s="14"/>
+      <c r="B112" s="14"/>
+      <c r="C112" s="15"/>
     </row>
     <row r="113" spans="1:3">
-      <c r="A113" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="C113" s="8" t="s">
-        <v>427</v>
-      </c>
+      <c r="A113" s="14"/>
+      <c r="B113" s="14"/>
+      <c r="C113" s="15"/>
     </row>
     <row r="114" spans="1:3">
-      <c r="A114" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="C114" s="8" t="s">
-        <v>428</v>
-      </c>
+      <c r="A114" s="14"/>
+      <c r="B114" s="14"/>
+      <c r="C114" s="15"/>
     </row>
     <row r="115" spans="1:3">
-      <c r="A115" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C115" s="8" t="s">
-        <v>429</v>
-      </c>
+      <c r="A115" s="14"/>
+      <c r="B115" s="14"/>
+      <c r="C115" s="15"/>
     </row>
     <row r="116" spans="1:3">
-      <c r="A116" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="C116" s="9">
-        <v>43641.105358796296</v>
-      </c>
+      <c r="A116" s="14"/>
+      <c r="B116" s="14"/>
+      <c r="C116" s="16"/>
     </row>
     <row r="117" spans="1:3">
-      <c r="A117" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="C117" s="8">
-        <v>1561429903</v>
-      </c>
+      <c r="A117" s="14"/>
+      <c r="B117" s="14"/>
+      <c r="C117" s="15"/>
     </row>
     <row r="118" spans="1:3">
-      <c r="A118" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="C118" s="8">
-        <v>1561429903.6035099</v>
-      </c>
+      <c r="A118" s="14"/>
+      <c r="B118" s="14"/>
+      <c r="C118" s="15"/>
     </row>
     <row r="119" spans="1:3">
-      <c r="A119" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="C119" s="8" t="s">
-        <v>322</v>
-      </c>
+      <c r="A119" s="14"/>
+      <c r="B119" s="14"/>
+      <c r="C119" s="15"/>
     </row>
     <row r="120" spans="1:3">
-      <c r="A120" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C120" s="8" t="s">
-        <v>324</v>
-      </c>
+      <c r="A120" s="14"/>
+      <c r="B120" s="14"/>
+      <c r="C120" s="15"/>
     </row>
     <row r="121" spans="1:3">
-      <c r="A121" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="C121" s="8" t="s">
-        <v>326</v>
-      </c>
+      <c r="A121" s="14"/>
+      <c r="B121" s="14"/>
+      <c r="C121" s="15"/>
     </row>
     <row r="122" spans="1:3">
-      <c r="A122" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="C122" s="8" t="s">
-        <v>328</v>
-      </c>
+      <c r="A122" s="14"/>
+      <c r="B122" s="14"/>
+      <c r="C122" s="15"/>
     </row>
     <row r="123" spans="1:3">
-      <c r="A123" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="C123" s="8" t="s">
-        <v>330</v>
-      </c>
+      <c r="A123" s="14"/>
+      <c r="B123" s="14"/>
+      <c r="C123" s="15"/>
     </row>
     <row r="124" spans="1:3">
-      <c r="A124" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="C124" s="8" t="s">
-        <v>332</v>
-      </c>
+      <c r="A124" s="14"/>
+      <c r="B124" s="14"/>
+      <c r="C124" s="15"/>
     </row>
     <row r="125" spans="1:3">
-      <c r="A125" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B125" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C125" s="8" t="s">
-        <v>334</v>
-      </c>
+      <c r="A125" s="14"/>
+      <c r="B125" s="14"/>
+      <c r="C125" s="15"/>
     </row>
     <row r="126" spans="1:3">
-      <c r="A126" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="C126" s="8">
-        <v>0</v>
-      </c>
+      <c r="A126" s="14"/>
+      <c r="B126" s="14"/>
+      <c r="C126" s="15"/>
     </row>
     <row r="127" spans="1:3">
-      <c r="A127" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="C127" s="8">
-        <v>1000</v>
-      </c>
+      <c r="A127" s="14"/>
+      <c r="B127" s="14"/>
+      <c r="C127" s="15"/>
     </row>
     <row r="128" spans="1:3">
-      <c r="A128" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="C128" s="8" t="s">
-        <v>338</v>
-      </c>
+      <c r="A128" s="14"/>
+      <c r="B128" s="14"/>
+      <c r="C128" s="15"/>
     </row>
     <row r="129" spans="1:3">
-      <c r="A129" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="C129" s="8">
-        <v>20</v>
-      </c>
+      <c r="A129" s="14"/>
+      <c r="B129" s="14"/>
+      <c r="C129" s="15"/>
     </row>
     <row r="130" spans="1:3">
-      <c r="A130" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B130" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="C130" s="8">
-        <v>10</v>
-      </c>
+      <c r="A130" s="14"/>
+      <c r="B130" s="14"/>
+      <c r="C130" s="15"/>
     </row>
     <row r="131" spans="1:3">
-      <c r="A131" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="C131" s="8">
-        <v>10</v>
-      </c>
+      <c r="A131" s="14"/>
+      <c r="B131" s="14"/>
+      <c r="C131" s="15"/>
     </row>
     <row r="132" spans="1:3">
-      <c r="A132" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="C132" s="8">
-        <v>4</v>
-      </c>
+      <c r="A132" s="14"/>
+      <c r="B132" s="14"/>
+      <c r="C132" s="15"/>
     </row>
     <row r="133" spans="1:3">
-      <c r="A133" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="C133" s="8" t="s">
-        <v>344</v>
-      </c>
+      <c r="A133" s="14"/>
+      <c r="B133" s="14"/>
+      <c r="C133" s="15"/>
     </row>
     <row r="134" spans="1:3">
-      <c r="A134" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="C134" s="8" t="s">
-        <v>345</v>
-      </c>
+      <c r="A134" s="14"/>
+      <c r="B134" s="14"/>
+      <c r="C134" s="15"/>
     </row>
     <row r="135" spans="1:3">
-      <c r="A135" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="C135" s="8" t="s">
-        <v>346</v>
-      </c>
+      <c r="A135" s="14"/>
+      <c r="B135" s="14"/>
+      <c r="C135" s="15"/>
     </row>
     <row r="136" spans="1:3">
-      <c r="A136" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="C136" s="8" t="s">
-        <v>347</v>
-      </c>
+      <c r="A136" s="14"/>
+      <c r="B136" s="14"/>
+      <c r="C136" s="15"/>
     </row>
     <row r="137" spans="1:3">
-      <c r="A137" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="C137" s="8" t="s">
-        <v>348</v>
-      </c>
+      <c r="A137" s="14"/>
+      <c r="B137" s="14"/>
+      <c r="C137" s="15"/>
     </row>
     <row r="138" spans="1:3">
-      <c r="A138" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B138" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="C138" s="8" t="s">
-        <v>350</v>
-      </c>
+      <c r="A138" s="14"/>
+      <c r="B138" s="14"/>
+      <c r="C138" s="15"/>
     </row>
     <row r="139" spans="1:3">
-      <c r="A139" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C139" s="8" t="s">
-        <v>352</v>
-      </c>
+      <c r="A139" s="14"/>
+      <c r="B139" s="14"/>
+      <c r="C139" s="15"/>
     </row>
     <row r="140" spans="1:3">
-      <c r="A140" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B140" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C140" s="8" t="s">
-        <v>353</v>
-      </c>
+      <c r="A140" s="14"/>
+      <c r="B140" s="14"/>
+      <c r="C140" s="15"/>
     </row>
     <row r="141" spans="1:3">
-      <c r="A141" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C141" s="8" t="s">
-        <v>354</v>
-      </c>
+      <c r="A141" s="14"/>
+      <c r="B141" s="14"/>
+      <c r="C141" s="15"/>
     </row>
     <row r="142" spans="1:3">
-      <c r="A142" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B142" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C142" s="8" t="s">
-        <v>430</v>
-      </c>
+      <c r="A142" s="14"/>
+      <c r="B142" s="14"/>
+      <c r="C142" s="15"/>
     </row>
     <row r="143" spans="1:3">
-      <c r="A143" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="B143" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C143" s="8" t="s">
-        <v>356</v>
-      </c>
+      <c r="A143" s="14"/>
+      <c r="B143" s="14"/>
+      <c r="C143" s="15"/>
     </row>
     <row r="144" spans="1:3">
-      <c r="A144" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="B144" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="C144" s="8" t="s">
-        <v>432</v>
-      </c>
+      <c r="A144" s="14"/>
+      <c r="B144" s="14"/>
+      <c r="C144" s="15"/>
     </row>
     <row r="145" spans="1:3">
-      <c r="A145" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="C145" s="8">
-        <v>1</v>
-      </c>
+      <c r="A145" s="14"/>
+      <c r="B145" s="14"/>
+      <c r="C145" s="15"/>
     </row>
     <row r="146" spans="1:3">
-      <c r="A146" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="C146" s="8" t="s">
-        <v>389</v>
-      </c>
+      <c r="A146" s="14"/>
+      <c r="B146" s="14"/>
+      <c r="C146" s="15"/>
     </row>
     <row r="147" spans="1:3">
-      <c r="A147" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="C147" s="8" t="s">
-        <v>389</v>
-      </c>
+      <c r="A147" s="14"/>
+      <c r="B147" s="14"/>
+      <c r="C147" s="15"/>
     </row>
     <row r="148" spans="1:3">
-      <c r="A148" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="C148" s="8" t="s">
-        <v>392</v>
-      </c>
+      <c r="A148" s="14"/>
+      <c r="B148" s="14"/>
+      <c r="C148" s="15"/>
     </row>
     <row r="149" spans="1:3">
-      <c r="A149" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="C149" s="9">
-        <v>43641.105358796296</v>
-      </c>
+      <c r="A149" s="14"/>
+      <c r="B149" s="14"/>
+      <c r="C149" s="16"/>
     </row>
     <row r="150" spans="1:3">
-      <c r="A150" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="C150" s="8">
-        <v>1561429903</v>
-      </c>
+      <c r="A150" s="14"/>
+      <c r="B150" s="14"/>
+      <c r="C150" s="15"/>
     </row>
     <row r="151" spans="1:3">
-      <c r="A151" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="C151" s="8">
-        <v>1561429903.6035099</v>
-      </c>
+      <c r="A151" s="14"/>
+      <c r="B151" s="14"/>
+      <c r="C151" s="15"/>
     </row>
     <row r="152" spans="1:3">
-      <c r="A152" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="C152" s="8">
-        <v>3</v>
-      </c>
+      <c r="A152" s="14"/>
+      <c r="B152" s="14"/>
+      <c r="C152" s="15"/>
     </row>
     <row r="153" spans="1:3">
-      <c r="A153" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="C153" s="8" t="s">
-        <v>399</v>
-      </c>
+      <c r="A153" s="14"/>
+      <c r="B153" s="14"/>
+      <c r="C153" s="15"/>
     </row>
     <row r="154" spans="1:3">
-      <c r="A154" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="C154" s="8" t="s">
-        <v>295</v>
-      </c>
+      <c r="A154" s="14"/>
+      <c r="B154" s="14"/>
+      <c r="C154" s="15"/>
     </row>
     <row r="155" spans="1:3">
-      <c r="A155" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="C155" s="8" t="s">
-        <v>297</v>
-      </c>
+      <c r="A155" s="1"/>
+      <c r="B155" s="1"/>
+      <c r="C155" s="8"/>
     </row>
     <row r="156" spans="1:3">
-      <c r="A156" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="C156" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="A156" s="1"/>
+      <c r="B156" s="1"/>
+      <c r="C156" s="8"/>
     </row>
     <row r="157" spans="1:3">
-      <c r="A157" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="C157" s="8" t="s">
-        <v>301</v>
-      </c>
+      <c r="A157" s="1"/>
+      <c r="B157" s="1"/>
+      <c r="C157" s="8"/>
     </row>
     <row r="158" spans="1:3">
-      <c r="A158" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="C158" s="8" t="s">
-        <v>303</v>
-      </c>
+      <c r="A158" s="1"/>
+      <c r="B158" s="1"/>
+      <c r="C158" s="8"/>
     </row>
     <row r="159" spans="1:3">
-      <c r="A159" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="B159" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="C159" s="8" t="s">
-        <v>305</v>
-      </c>
+      <c r="A159" s="1"/>
+      <c r="B159" s="1"/>
+      <c r="C159" s="8"/>
     </row>
     <row r="160" spans="1:3">
-      <c r="A160" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="C160" s="8" t="s">
-        <v>307</v>
-      </c>
+      <c r="A160" s="1"/>
+      <c r="B160" s="1"/>
+      <c r="C160" s="8"/>
     </row>
     <row r="161" spans="1:3">
-      <c r="A161" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="C161" s="8" t="s">
-        <v>309</v>
-      </c>
+      <c r="A161" s="1"/>
+      <c r="B161" s="1"/>
+      <c r="C161" s="8"/>
     </row>
     <row r="162" spans="1:3">
-      <c r="A162" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="C162" s="8" t="s">
-        <v>311</v>
-      </c>
+      <c r="A162" s="1"/>
+      <c r="B162" s="1"/>
+      <c r="C162" s="8"/>
     </row>
     <row r="163" spans="1:3">
-      <c r="A163" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="C163" s="8" t="s">
-        <v>426</v>
-      </c>
+      <c r="A163" s="1"/>
+      <c r="B163" s="1"/>
+      <c r="C163" s="8"/>
     </row>
     <row r="164" spans="1:3">
-      <c r="A164" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="C164" s="8" t="s">
-        <v>427</v>
-      </c>
+      <c r="A164" s="1"/>
+      <c r="B164" s="1"/>
+      <c r="C164" s="8"/>
     </row>
     <row r="165" spans="1:3">
-      <c r="A165" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B165" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="C165" s="8" t="s">
-        <v>428</v>
-      </c>
+      <c r="A165" s="1"/>
+      <c r="B165" s="1"/>
+      <c r="C165" s="8"/>
     </row>
     <row r="166" spans="1:3">
-      <c r="A166" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C166" s="8" t="s">
-        <v>429</v>
-      </c>
+      <c r="A166" s="1"/>
+      <c r="B166" s="1"/>
+      <c r="C166" s="8"/>
     </row>
     <row r="167" spans="1:3">
-      <c r="A167" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="C167" s="9">
-        <v>43641.105358796296</v>
-      </c>
+      <c r="A167" s="1"/>
+      <c r="B167" s="1"/>
+      <c r="C167" s="9"/>
     </row>
     <row r="168" spans="1:3">
-      <c r="A168" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="C168" s="8">
-        <v>1561429903</v>
-      </c>
+      <c r="A168" s="1"/>
+      <c r="B168" s="1"/>
+      <c r="C168" s="8"/>
     </row>
     <row r="169" spans="1:3">
-      <c r="A169" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="C169" s="8">
-        <v>1561429903.6035099</v>
-      </c>
+      <c r="A169" s="1"/>
+      <c r="B169" s="1"/>
+      <c r="C169" s="8"/>
     </row>
     <row r="170" spans="1:3">
-      <c r="A170" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="C170" s="8" t="s">
-        <v>322</v>
-      </c>
+      <c r="A170" s="1"/>
+      <c r="B170" s="1"/>
+      <c r="C170" s="8"/>
     </row>
     <row r="171" spans="1:3">
-      <c r="A171" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C171" s="8" t="s">
-        <v>324</v>
-      </c>
+      <c r="A171" s="1"/>
+      <c r="B171" s="1"/>
+      <c r="C171" s="8"/>
     </row>
     <row r="172" spans="1:3">
-      <c r="A172" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="C172" s="8" t="s">
-        <v>326</v>
-      </c>
+      <c r="A172" s="1"/>
+      <c r="B172" s="1"/>
+      <c r="C172" s="8"/>
     </row>
     <row r="173" spans="1:3">
-      <c r="A173" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="B173" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="C173" s="8" t="s">
-        <v>328</v>
-      </c>
+      <c r="A173" s="1"/>
+      <c r="B173" s="1"/>
+      <c r="C173" s="8"/>
     </row>
     <row r="174" spans="1:3">
-      <c r="A174" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="C174" s="8" t="s">
-        <v>330</v>
-      </c>
+      <c r="A174" s="1"/>
+      <c r="B174" s="1"/>
+      <c r="C174" s="8"/>
     </row>
     <row r="175" spans="1:3">
-      <c r="A175" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="C175" s="8" t="s">
-        <v>332</v>
-      </c>
+      <c r="A175" s="1"/>
+      <c r="B175" s="1"/>
+      <c r="C175" s="8"/>
     </row>
     <row r="176" spans="1:3">
-      <c r="A176" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="B176" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C176" s="8" t="s">
-        <v>334</v>
-      </c>
+      <c r="A176" s="1"/>
+      <c r="B176" s="1"/>
+      <c r="C176" s="8"/>
     </row>
     <row r="177" spans="1:3">
-      <c r="A177" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B177" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="C177" s="8">
-        <v>0</v>
-      </c>
+      <c r="A177" s="1"/>
+      <c r="B177" s="1"/>
+      <c r="C177" s="8"/>
     </row>
     <row r="178" spans="1:3">
-      <c r="A178" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="C178" s="8">
-        <v>1000</v>
-      </c>
+      <c r="A178" s="1"/>
+      <c r="B178" s="1"/>
+      <c r="C178" s="8"/>
     </row>
     <row r="179" spans="1:3">
-      <c r="A179" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="C179" s="8" t="s">
-        <v>338</v>
-      </c>
+      <c r="A179" s="1"/>
+      <c r="B179" s="1"/>
+      <c r="C179" s="8"/>
     </row>
     <row r="180" spans="1:3">
-      <c r="A180" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="C180" s="8">
-        <v>20</v>
-      </c>
+      <c r="A180" s="1"/>
+      <c r="B180" s="1"/>
+      <c r="C180" s="8"/>
     </row>
     <row r="181" spans="1:3">
-      <c r="A181" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="B181" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="C181" s="8">
-        <v>10</v>
-      </c>
+      <c r="A181" s="1"/>
+      <c r="B181" s="1"/>
+      <c r="C181" s="8"/>
     </row>
     <row r="182" spans="1:3">
-      <c r="A182" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="B182" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="C182" s="8">
-        <v>10</v>
-      </c>
+      <c r="A182" s="1"/>
+      <c r="B182" s="1"/>
+      <c r="C182" s="8"/>
     </row>
     <row r="183" spans="1:3">
-      <c r="A183" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="B183" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="C183" s="8">
-        <v>4</v>
-      </c>
+      <c r="A183" s="1"/>
+      <c r="B183" s="1"/>
+      <c r="C183" s="8"/>
     </row>
     <row r="184" spans="1:3">
-      <c r="A184" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="B184" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="C184" s="8" t="s">
-        <v>344</v>
-      </c>
+      <c r="A184" s="1"/>
+      <c r="B184" s="1"/>
+      <c r="C184" s="8"/>
     </row>
     <row r="185" spans="1:3">
-      <c r="A185" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="B185" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="C185" s="8" t="s">
-        <v>345</v>
-      </c>
+      <c r="A185" s="1"/>
+      <c r="B185" s="1"/>
+      <c r="C185" s="8"/>
     </row>
     <row r="186" spans="1:3">
-      <c r="A186" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="B186" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="C186" s="8" t="s">
-        <v>346</v>
-      </c>
+      <c r="A186" s="1"/>
+      <c r="B186" s="1"/>
+      <c r="C186" s="8"/>
     </row>
     <row r="187" spans="1:3">
-      <c r="A187" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="B187" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="C187" s="8" t="s">
-        <v>347</v>
-      </c>
+      <c r="A187" s="1"/>
+      <c r="B187" s="1"/>
+      <c r="C187" s="8"/>
     </row>
     <row r="188" spans="1:3">
-      <c r="A188" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B188" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="C188" s="8" t="s">
-        <v>348</v>
-      </c>
+      <c r="A188" s="1"/>
+      <c r="B188" s="1"/>
+      <c r="C188" s="8"/>
     </row>
     <row r="189" spans="1:3">
-      <c r="A189" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="B189" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="C189" s="8" t="s">
-        <v>350</v>
-      </c>
+      <c r="A189" s="1"/>
+      <c r="B189" s="1"/>
+      <c r="C189" s="8"/>
     </row>
     <row r="190" spans="1:3">
-      <c r="A190" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="B190" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C190" s="8" t="s">
-        <v>352</v>
-      </c>
+      <c r="A190" s="1"/>
+      <c r="B190" s="1"/>
+      <c r="C190" s="8"/>
     </row>
     <row r="191" spans="1:3">
-      <c r="A191" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="B191" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C191" s="8" t="s">
-        <v>353</v>
-      </c>
+      <c r="A191" s="1"/>
+      <c r="B191" s="1"/>
+      <c r="C191" s="8"/>
     </row>
     <row r="192" spans="1:3">
-      <c r="A192" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="B192" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C192" s="8" t="s">
-        <v>354</v>
-      </c>
+      <c r="A192" s="1"/>
+      <c r="B192" s="1"/>
+      <c r="C192" s="8"/>
     </row>
     <row r="193" spans="1:3">
-      <c r="A193" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="B193" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C193" s="8" t="s">
-        <v>430</v>
-      </c>
+      <c r="A193" s="1"/>
+      <c r="B193" s="1"/>
+      <c r="C193" s="8"/>
     </row>
     <row r="194" spans="1:3">
-      <c r="A194" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="B194" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C194" s="8" t="s">
-        <v>356</v>
-      </c>
+      <c r="A194" s="1"/>
+      <c r="B194" s="1"/>
+      <c r="C194" s="8"/>
     </row>
     <row r="195" spans="1:3">
-      <c r="A195" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="B195" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="C195" s="8" t="s">
-        <v>432</v>
-      </c>
+      <c r="A195" s="1"/>
+      <c r="B195" s="1"/>
+      <c r="C195" s="8"/>
     </row>
     <row r="196" spans="1:3">
-      <c r="A196" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="B196" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="C196" s="8">
-        <v>1</v>
-      </c>
+      <c r="A196" s="1"/>
+      <c r="B196" s="1"/>
+      <c r="C196" s="8"/>
     </row>
     <row r="197" spans="1:3">
-      <c r="A197" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="B197" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="C197" s="8" t="s">
-        <v>389</v>
-      </c>
+      <c r="A197" s="1"/>
+      <c r="B197" s="1"/>
+      <c r="C197" s="8"/>
     </row>
     <row r="198" spans="1:3">
-      <c r="A198" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B198" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="C198" s="8" t="s">
-        <v>389</v>
-      </c>
+      <c r="A198" s="1"/>
+      <c r="B198" s="1"/>
+      <c r="C198" s="8"/>
     </row>
     <row r="199" spans="1:3">
-      <c r="A199" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="B199" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="C199" s="8" t="s">
-        <v>392</v>
-      </c>
+      <c r="A199" s="1"/>
+      <c r="B199" s="1"/>
+      <c r="C199" s="8"/>
     </row>
     <row r="200" spans="1:3">
-      <c r="A200" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="B200" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="C200" s="9">
-        <v>43641.105358796296</v>
-      </c>
+      <c r="A200" s="1"/>
+      <c r="B200" s="1"/>
+      <c r="C200" s="9"/>
     </row>
     <row r="201" spans="1:3">
-      <c r="A201" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="B201" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="C201" s="8">
-        <v>1561429903</v>
-      </c>
+      <c r="A201" s="1"/>
+      <c r="B201" s="1"/>
+      <c r="C201" s="8"/>
     </row>
     <row r="202" spans="1:3">
-      <c r="A202" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="B202" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="C202" s="8">
-        <v>1561429903.6035099</v>
-      </c>
+      <c r="A202" s="1"/>
+      <c r="B202" s="1"/>
+      <c r="C202" s="8"/>
     </row>
     <row r="203" spans="1:3">
-      <c r="A203" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="B203" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="C203" s="8">
-        <v>3</v>
-      </c>
+      <c r="A203" s="1"/>
+      <c r="B203" s="1"/>
+      <c r="C203" s="8"/>
     </row>
     <row r="204" spans="1:3">
-      <c r="A204" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="B204" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="C204" s="8" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3">
-      <c r="A205" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B205" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="C205" s="8" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3">
-      <c r="A206" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B206" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="C206" s="8"/>
-    </row>
-    <row r="207" spans="1:3">
-      <c r="A207" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B207" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="C207" s="8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3">
-      <c r="A208" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B208" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="C208" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3">
-      <c r="A209" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B209" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="C209" s="8" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3">
-      <c r="A210" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B210" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="C210" s="8" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3">
-      <c r="A211" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B211" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="C211" s="8" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3">
-      <c r="A212" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B212" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="C212" s="8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3">
-      <c r="A213" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B213" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="C213" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3">
-      <c r="A214" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B214" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="C214" s="8" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3">
-      <c r="A215" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B215" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="C215" s="8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3">
-      <c r="A216" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B216" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="C216" s="8" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3">
-      <c r="A217" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B217" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="C217" s="8" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3">
-      <c r="A218" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B218" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="C218" s="8" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3">
-      <c r="A219" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B219" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="C219" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3">
-      <c r="A220" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="B220" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="C220" s="8" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3">
-      <c r="A221" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B221" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="C221" s="8" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3">
-      <c r="A222" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B222" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="C222" s="10">
-        <v>36892</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3">
-      <c r="A223" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B223" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="C223" s="8" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3">
-      <c r="A224" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B224" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="C224" s="8" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3">
-      <c r="A225" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="B225" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="C225" s="8" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3">
-      <c r="A226" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B226" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="C226" s="8" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3">
-      <c r="A227" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B227" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="C227" s="9">
-        <v>43641.105358796296</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3">
-      <c r="A228" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B228" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="C228" s="8">
-        <v>1561429903</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3">
-      <c r="A229" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B229" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="C229" s="8">
-        <v>1561429903.6035099</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3" ht="195">
-      <c r="A230" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="B230" s="13" t="s">
-        <v>425</v>
-      </c>
-      <c r="C230" s="12" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3">
-      <c r="A231" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B231" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="C231" s="8" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3">
-      <c r="A232" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B232" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="C232" s="8">
-        <v>299000</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3">
-      <c r="A233" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B233" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C233" s="8">
-        <v>30290121</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3">
-      <c r="A234" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B234" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="C234" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3">
-      <c r="A235" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B235" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="C235" s="8">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3">
-      <c r="A236" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B236" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="C236" s="8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3">
-      <c r="A237" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B237" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="C237" s="8">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3">
-      <c r="A238" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B238" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="C238" s="8">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3">
-      <c r="A239" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B239" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="C239" s="8" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3">
-      <c r="A240" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B240" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="C240" s="8" t="s">
-        <v>422</v>
-      </c>
+      <c r="A204" s="1"/>
+      <c r="B204" s="1"/>
+      <c r="C204" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>